<commit_message>
Add additional AllProductsPage tests
</commit_message>
<xml_diff>
--- a/src/test/java/com/github/jacoberson/utilities/excelFiles/ExcelTest.xlsx
+++ b/src/test/java/com/github/jacoberson/utilities/excelFiles/ExcelTest.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15802\seleniumpractice\SauceDemoPOM\src\test\resources\utilities\excelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15802\seleniumpractice\SauceDemoPOM\src\test\java\com\github\jacoberson\utilities\excelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434FA85F-EEAC-4128-945C-7CA17CD0025E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2569AE98-9BD7-426B-B229-20B8A4CF505D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34905" yWindow="8715" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32550" yWindow="2265" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="validateLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="verifyLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="verifyAddAndRemoveButtons" sheetId="3" r:id="rId2"/>
+    <sheet name="verifyItemSort" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>username</t>
   </si>
@@ -52,6 +54,81 @@
   </si>
   <si>
     <t>Epic sadface: Password is required</t>
+  </si>
+  <si>
+    <t>itemsToAdd</t>
+  </si>
+  <si>
+    <t>Sauce Labs Backpack</t>
+  </si>
+  <si>
+    <t>Sauce Labs Bolt T-Shirt, Sauce Labs Backpack, Test.allTheThings() T-Shirt (Red)</t>
+  </si>
+  <si>
+    <t>Sauce Labs Backpack, Sauce Labs Bike Light, Sauce Labs Bolt T-Shirt, Sauce Labs Fleece Jacket, Sauce Labs Onesie, Test.allTheThings() T-Shirt (Red)</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>itemsToRemove</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Sauce Labs Bolt T-Shirt, Test.allTheThings() T-Shirt (Red)</t>
+  </si>
+  <si>
+    <t>addButtonCount</t>
+  </si>
+  <si>
+    <t>removeButtonCount</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Sauce Labs Bike Light, Sauce Labs Bolt T-Shirt, Test.allTheThings() T-Shirt (Red)</t>
+  </si>
+  <si>
+    <t>sortType</t>
+  </si>
+  <si>
+    <t>firstItem</t>
+  </si>
+  <si>
+    <t>lastItem</t>
+  </si>
+  <si>
+    <t>Name (Z to A)</t>
+  </si>
+  <si>
+    <t>Price (low to high)</t>
+  </si>
+  <si>
+    <t>Price (high to low)</t>
+  </si>
+  <si>
+    <t>Name (A to Z)</t>
+  </si>
+  <si>
+    <t>Test.allTheThings() T-Shirt (Red)</t>
+  </si>
+  <si>
+    <t>Sauce Labs Onesie</t>
+  </si>
+  <si>
+    <t>Sauce Labs Fleece Jacket</t>
+  </si>
+  <si>
+    <t>cartCount</t>
   </si>
 </sst>
 </file>
@@ -87,8 +164,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,4 +514,169 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC1C912-3A4A-49E5-96A5-02FE59ED6414}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="132.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4926DBF0-9C5A-46F2-B86C-6CE9CF38CF94}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update excel file to include SingleProductPage test
</commit_message>
<xml_diff>
--- a/src/test/java/com/github/jacoberson/utilities/excelFiles/ExcelTest.xlsx
+++ b/src/test/java/com/github/jacoberson/utilities/excelFiles/ExcelTest.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15802\seleniumpractice\SauceDemoPOM\src\test\java\com\github\jacoberson\utilities\excelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2569AE98-9BD7-426B-B229-20B8A4CF505D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84FB8E9-3C9A-4950-AC40-443F1EE817D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32550" yWindow="2265" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32145" yWindow="6240" windowWidth="20970" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="verifyLogin" sheetId="1" r:id="rId1"/>
     <sheet name="verifyAddAndRemoveButtons" sheetId="3" r:id="rId2"/>
     <sheet name="verifyItemSort" sheetId="4" r:id="rId3"/>
+    <sheet name="verifyCanOpenItemDetailsPage" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>username</t>
   </si>
@@ -129,6 +130,24 @@
   </si>
   <si>
     <t>cartCount</t>
+  </si>
+  <si>
+    <t>itemName</t>
+  </si>
+  <si>
+    <t>Sauce Labs Bolt T-Shirt</t>
+  </si>
+  <si>
+    <t>itemUrl</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/inventory-item.html?id=4</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/inventory-item.html?id=3</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/inventory-item.html?id=1</t>
   </si>
 </sst>
 </file>
@@ -520,7 +539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC1C912-3A4A-49E5-96A5-02FE59ED6414}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -679,4 +698,52 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E296B54-647E-4D89-8C33-935980012D6A}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
WebCoreDriver eager instantiation & social media method
Changed WebCoreDriver singleton class to eager instantiation and
consolidated Twitter & Facebook tests to a single social media test
</commit_message>
<xml_diff>
--- a/src/test/java/com/github/jacoberson/utilities/excelFiles/ExcelTest.xlsx
+++ b/src/test/java/com/github/jacoberson/utilities/excelFiles/ExcelTest.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15802\seleniumpractice\SauceDemoPOM\src\test\java\com\github\jacoberson\utilities\excelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84FB8E9-3C9A-4950-AC40-443F1EE817D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0622B009-CA06-4D48-95BD-1F30BCED8EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32145" yWindow="6240" windowWidth="20970" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33750" yWindow="3735" windowWidth="20970" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="verifyLogin" sheetId="1" r:id="rId1"/>
     <sheet name="verifyAddAndRemoveButtons" sheetId="3" r:id="rId2"/>
     <sheet name="verifyItemSort" sheetId="4" r:id="rId3"/>
-    <sheet name="verifyCanOpenItemDetailsPage" sheetId="5" r:id="rId4"/>
+    <sheet name="verifySocialMediaLinks" sheetId="6" r:id="rId4"/>
+    <sheet name="verifyCanOpenItemDetailsPage" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>username</t>
   </si>
@@ -148,6 +149,24 @@
   </si>
   <si>
     <t>https://www.saucedemo.com/inventory-item.html?id=1</t>
+  </si>
+  <si>
+    <t>https://twitter.com/saucelabs</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/saucelabs</t>
+  </si>
+  <si>
+    <t>socialMediaUrl</t>
+  </si>
+  <si>
+    <t>socialMediaSite</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>Facebook</t>
   </si>
 </sst>
 </file>
@@ -701,10 +720,49 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC0AAE13-5148-44B1-937E-D05D96C560CD}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E296B54-647E-4D89-8C33-935980012D6A}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add CheckoutStepOne page object, elements, assertions, and tests
</commit_message>
<xml_diff>
--- a/src/test/java/com/github/jacoberson/utilities/excelFiles/ExcelTest.xlsx
+++ b/src/test/java/com/github/jacoberson/utilities/excelFiles/ExcelTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15802\seleniumpractice\SauceDemoPOM\src\test\java\com\github\jacoberson\utilities\excelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0622B009-CA06-4D48-95BD-1F30BCED8EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7A5E55-37BB-4B62-9294-30E9AA113D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33750" yWindow="3735" windowWidth="20970" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33570" yWindow="2790" windowWidth="20970" windowHeight="11385" tabRatio="618" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="verifyLogin" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="verifyItemSort" sheetId="4" r:id="rId3"/>
     <sheet name="verifySocialMediaLinks" sheetId="6" r:id="rId4"/>
     <sheet name="verifyCanOpenItemDetailsPage" sheetId="5" r:id="rId5"/>
+    <sheet name="verifyCartItemsDisplayCorrectly" sheetId="7" r:id="rId6"/>
+    <sheet name="verifyCartItemsCanBeRemoved" sheetId="8" r:id="rId7"/>
+    <sheet name="verifyCheckoutInformation" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
   <si>
     <t>username</t>
   </si>
@@ -167,6 +170,45 @@
   </si>
   <si>
     <t>Facebook</t>
+  </si>
+  <si>
+    <t>Sauce Labs Fleece Jacket, Sauce Labs Bolt T-Shirt, Test.allTheThings() T-Shirt (Red)</t>
+  </si>
+  <si>
+    <t>Sauce Labs Backpack, Sauce Labs Bike Light, Sauce Labs Bolt T-Shirt, Sauce Labs Onesie, Test.allTheThings() T-Shirt (Red)</t>
+  </si>
+  <si>
+    <t>itemCount</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Sauce Labs Backpack, Sauce Labs Bolt T-Shirt, Sauce Labs Onesie, Test.allTheThings() T-Shirt (Red)</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>zipCode</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Error: First Name is required</t>
+  </si>
+  <si>
+    <t>Error: Last Name is required</t>
+  </si>
+  <si>
+    <t>Error: Postal Code is required</t>
   </si>
 </sst>
 </file>
@@ -558,7 +600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC1C912-3A4A-49E5-96A5-02FE59ED6414}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -723,7 +765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC0AAE13-5148-44B1-937E-D05D96C560CD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -804,4 +846,199 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB449B1-1A78-4D9D-B53B-61D96723B225}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="109" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEA5286-7990-4730-B4F7-EC1ADC505C03}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="109" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20CC6C25-1291-4B8C-A8C6-0905D6967B36}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3">
+        <v>12345</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4">
+        <v>12345</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add CheckoutStepTwo calculate methods
</commit_message>
<xml_diff>
--- a/src/test/java/com/github/jacoberson/utilities/excelFiles/ExcelTest.xlsx
+++ b/src/test/java/com/github/jacoberson/utilities/excelFiles/ExcelTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15802\seleniumpractice\SauceDemoPOM\src\test\java\com\github\jacoberson\utilities\excelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7A5E55-37BB-4B62-9294-30E9AA113D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BBBE48-994E-4887-A40C-A2C1C04FEEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33570" yWindow="2790" windowWidth="20970" windowHeight="11385" tabRatio="618" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5820" yWindow="2205" windowWidth="20970" windowHeight="11385" tabRatio="618" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="verifyLogin" sheetId="1" r:id="rId1"/>
@@ -969,7 +969,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Extract some repeated commands to single method
</commit_message>
<xml_diff>
--- a/src/test/java/com/github/jacoberson/utilities/excelFiles/ExcelTest.xlsx
+++ b/src/test/java/com/github/jacoberson/utilities/excelFiles/ExcelTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15802\seleniumpractice\SauceDemoPOM\src\test\java\com\github\jacoberson\utilities\excelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BBBE48-994E-4887-A40C-A2C1C04FEEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682C9115-18CF-4877-85C4-C8D47D8519C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="2205" windowWidth="20970" windowHeight="11385" tabRatio="618" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="618" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="verifyLogin" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="verifyCartItemsDisplayCorrectly" sheetId="7" r:id="rId6"/>
     <sheet name="verifyCartItemsCanBeRemoved" sheetId="8" r:id="rId7"/>
     <sheet name="verifyCheckoutInformation" sheetId="9" r:id="rId8"/>
+    <sheet name="verifyCheckoutOverview" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
   <si>
     <t>username</t>
   </si>
@@ -905,7 +906,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20CC6C25-1291-4B8C-A8C6-0905D6967B36}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,4 +1042,42 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DA3C30-1740-4C59-A990-0660F4AB6003}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="109" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>